<commit_message>
added hymenoptera summary results
</commit_message>
<xml_diff>
--- a/data/summary.xlsx
+++ b/data/summary.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37920" windowHeight="25120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37920" windowHeight="25120" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad2" sheetId="2" r:id="rId1"/>
+    <sheet name="Araneae" sheetId="2" r:id="rId1"/>
+    <sheet name="Hymenoptera" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="138">
   <si>
     <t>bin</t>
   </si>
@@ -421,6 +422,18 @@
   </si>
   <si>
     <t>BOLD:AAC0342</t>
+  </si>
+  <si>
+    <t>BOLD:AAA1223</t>
+  </si>
+  <si>
+    <t>BOLD:AAA1257</t>
+  </si>
+  <si>
+    <t>BOLD:AAA1258</t>
+  </si>
+  <si>
+    <t>BOLD:AAA1265</t>
   </si>
 </sst>
 </file>
@@ -507,7 +520,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Blad2!$C$2:$C$132</c:f>
+              <c:f>Araneae!$C$2:$C$132</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="131"/>
@@ -909,7 +922,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad2!$B$2:$B$132</c:f>
+              <c:f>Araneae!$B$2:$B$132</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="131"/>
@@ -1319,11 +1332,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2086377400"/>
-        <c:axId val="2086360232"/>
+        <c:axId val="2122366872"/>
+        <c:axId val="2122362520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2086377400"/>
+        <c:axId val="2122366872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,12 +1346,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086360232"/>
+        <c:crossAx val="2122362520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2086360232"/>
+        <c:axId val="2122362520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.02"/>
@@ -1350,7 +1363,148 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086377400"/>
+        <c:crossAx val="2122366872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hymenoptera!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-85.3620125000249</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-80.10744105260549</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-80.10744105260549</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-85.2398586466482</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hymenoptera!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.00183070809572035</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00240035171994709</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00240035171994709</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>9.82190145342305E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2130150280"/>
+        <c:axId val="2130148856"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2130150280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2130148856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2130148856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2130150280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1386,6 +1540,41 @@
       <xdr:colOff>584200</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1731,7 +1920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C132"/>
     </sheetView>
   </sheetViews>
@@ -3187,6 +3376,82 @@
       </c>
       <c r="C132">
         <v>51.783444444444399</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2">
+        <v>1.83070809572035E-3</v>
+      </c>
+      <c r="C2">
+        <v>-85.362012500024903</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3">
+        <v>2.40035171994709E-3</v>
+      </c>
+      <c r="C3">
+        <v>-80.107441052605495</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4">
+        <v>2.40035171994709E-3</v>
+      </c>
+      <c r="C4">
+        <v>-80.107441052605495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9.8219014534230498E-5</v>
+      </c>
+      <c r="C5">
+        <v>-85.239858646648202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>